<commit_message>
Cleaning and formatting graphs
</commit_message>
<xml_diff>
--- a/Data/4_MD_LU_2025_2055.xlsx
+++ b/Data/4_MD_LU_2025_2055.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Data_Projects\States\MD\TechnicalForests\Data\Task5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UVM\Maryland_Technical_Forest\MD_Forest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0834B1DB-88CF-45DD-9AE4-55A00409D093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E54D034-A782-4789-9C36-6DA0A8727588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2025" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>FIPS</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>PAS_25-55</t>
+  </si>
+  <si>
+    <t>BALTIMORE CITY</t>
   </si>
 </sst>
 </file>
@@ -2814,7 +2817,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3880,7 +3883,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B25">
         <v>24510</v>

</xml_diff>